<commit_message>
added hours for monday and tuesday.
</commit_message>
<xml_diff>
--- a/docs/CS297_TimeTracking .xlsx
+++ b/docs/CS297_TimeTracking .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G\Desktop\Capstone Spring 2021\Thrillful\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE35AF8-24F0-4B27-86E4-0926DE1D540C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EDB31A-A22E-4358-A173-5830F5992BFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,11 +559,11 @@
       </c>
       <c r="D4">
         <f>'Week 1'!E$10</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="E4">
         <f>D4</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F4">
         <f>'Week 1'!G$10</f>
@@ -600,7 +600,7 @@
       </c>
       <c r="E5">
         <f>D5+E4</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F5">
         <f>'Week 2'!G$10</f>
@@ -637,7 +637,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F6">
         <f>'Week 3'!G$10</f>
@@ -674,7 +674,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F7">
         <f>'Week 4'!G$10</f>
@@ -711,7 +711,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F8">
         <f>'Week 5'!G$10</f>
@@ -748,7 +748,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F9">
         <f>'Week 6'!G$10</f>
@@ -785,7 +785,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F10">
         <f>'Week 7'!G$10</f>
@@ -822,7 +822,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F11">
         <f>'Week 8'!G$10</f>
@@ -859,7 +859,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F12">
         <f>'Week 9'!G$10</f>
@@ -896,7 +896,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F13">
         <f>'Week 10'!G$10</f>
@@ -1443,7 +1443,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1513,10 +1513,12 @@
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
       <c r="E4">
         <f>D4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4">
@@ -1538,10 +1540,12 @@
         <f>B5+C4</f>
         <v>0</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>4.5</v>
+      </c>
       <c r="E5">
         <f>D5+E4</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5">
@@ -1566,7 +1570,7 @@
       <c r="D6" s="1"/>
       <c r="E6">
         <f>D6+E5</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
@@ -1591,7 +1595,7 @@
       <c r="D7" s="1"/>
       <c r="E7">
         <f>D7+E6</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
@@ -1616,7 +1620,7 @@
       <c r="D8" s="1"/>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8">
@@ -1641,7 +1645,7 @@
       <c r="D9" s="1"/>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9">
@@ -1666,7 +1670,7 @@
       <c r="D10" s="1"/>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10">

</xml_diff>

<commit_message>
colab docs, team agreement
</commit_message>
<xml_diff>
--- a/docs/CS297_TimeTracking .xlsx
+++ b/docs/CS297_TimeTracking .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G\Desktop\Capstone Spring 2021\Thrillful\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F37FF4-D717-44F4-A471-01FDA21D5B01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867FE21E-CA7F-428B-B768-1EBB13F0E9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="1" r:id="rId1"/>
@@ -559,11 +559,11 @@
       </c>
       <c r="D4">
         <f>'Week 1'!E$10</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="E4">
         <f>D4</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F4">
         <f>'Week 1'!G$10</f>
@@ -600,7 +600,7 @@
       </c>
       <c r="E5">
         <f>D5+E4</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F5">
         <f>'Week 2'!G$10</f>
@@ -637,7 +637,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F6">
         <f>'Week 3'!G$10</f>
@@ -674,7 +674,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F7">
         <f>'Week 4'!G$10</f>
@@ -711,7 +711,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F8">
         <f>'Week 5'!G$10</f>
@@ -748,7 +748,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F9">
         <f>'Week 6'!G$10</f>
@@ -785,7 +785,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F10">
         <f>'Week 7'!G$10</f>
@@ -822,7 +822,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F11">
         <f>'Week 8'!G$10</f>
@@ -859,7 +859,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F12">
         <f>'Week 9'!G$10</f>
@@ -896,7 +896,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F13">
         <f>'Week 10'!G$10</f>
@@ -1443,7 +1443,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1567,10 +1567,12 @@
         <f>B6+C5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
       <c r="E6">
         <f>D6+E5</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
@@ -1595,7 +1597,7 @@
       <c r="D7" s="1"/>
       <c r="E7">
         <f>D7+E6</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
@@ -1620,7 +1622,7 @@
       <c r="D8" s="1"/>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8">
@@ -1645,7 +1647,7 @@
       <c r="D9" s="1"/>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9">
@@ -1670,7 +1672,7 @@
       <c r="D10" s="1"/>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10">

</xml_diff>